<commit_message>
Ready Labs and products data
</commit_message>
<xml_diff>
--- a/data/labs_and_products.xlsx
+++ b/data/labs_and_products.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="labs" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="optimals" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ideals" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="products" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="ideales" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -1735,7 +1735,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Comma [0]" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1816,14 +1816,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.42105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0283400809717"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.6396761133603"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="66.0931174089069"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="66.6275303643725"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -2554,15 +2554,15 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.41295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -3054,20 +3054,21 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.40485829959514"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8704453441296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.74898785425101"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7894736842105"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -15430,13 +15431,13 @@
   </sheetPr>
   <dimension ref="B1:N12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>